<commit_message>
update week report and conference report
</commit_message>
<xml_diff>
--- a/showmecoo-web-docs/src/main/resources/周报/项目周报.xlsx
+++ b/showmecoo-web-docs/src/main/resources/周报/项目周报.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
   <si>
     <t>showmecoo工作计划模版</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -210,6 +210,14 @@
   </si>
   <si>
     <t>UI和VI设计修改1版</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>微信客户端界面Mock图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>魏鑫</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -702,10 +710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1009,6 +1017,17 @@
       </c>
       <c r="I16" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="7:9">
+      <c r="G17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" s="3">
+        <v>20160710</v>
+      </c>
+      <c r="I17" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>